<commit_message>
maintalk -> talk로 변경
</commit_message>
<xml_diff>
--- a/Project_V/Assets/ExcelFiles/dialogue_new.xlsx
+++ b/Project_V/Assets/ExcelFiles/dialogue_new.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr codeName="현재_통합_문서"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tksth\Desktop\Project_V\Project_V\Assets\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81318A70-6A80-4764-97D8-DB981E7A9728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9AC2F10-B920-448B-9E07-687ADF1B1F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{461F5768-34F7-45FC-8921-4FFC2D7E081A}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="71">
   <si>
     <t>Index</t>
   </si>
@@ -176,10 +176,6 @@
     <t>Test_Street</t>
   </si>
   <si>
-    <t>main_talk</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>MainTalk_Sprite</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -260,14 +256,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>chr1_image</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>chr2_image</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>chr1_image_change</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -294,6 +282,12 @@
   <si>
     <t>주인공의 말하기 1, 다음번에 단일 오더로 움직이기</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>chr1_image_change</t>
+  </si>
+  <si>
+    <t>chr2_image_change</t>
   </si>
 </sst>
 </file>
@@ -1302,7 +1296,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1325,7 +1319,7 @@
         <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -1334,25 +1328,25 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -1372,10 +1366,10 @@
       <c r="F2" s="4"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -1399,10 +1393,10 @@
       <c r="F3" s="4"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -1417,17 +1411,17 @@
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
         <v>27</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="3"/>
@@ -1451,7 +1445,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3" t="b">
@@ -1480,7 +1474,7 @@
         <v>3</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -1498,17 +1492,17 @@
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
         <v>27</v>
       </c>
       <c r="F7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="3"/>
@@ -1557,7 +1551,7 @@
         <v>4</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -1582,7 +1576,7 @@
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
@@ -1611,7 +1605,7 @@
         <v>5</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -1638,7 +1632,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3" t="b">
@@ -1664,10 +1658,10 @@
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -1694,7 +1688,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3" t="b">
@@ -1722,10 +1716,10 @@
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -1747,10 +1741,10 @@
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -1929,10 +1923,10 @@
       <c r="F23" s="4"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -1958,10 +1952,10 @@
       <c r="F24" s="4"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>

</xml_diff>